<commit_message>
create webhook swagger and refactoring some code
</commit_message>
<xml_diff>
--- a/public/template-import-faq-answers.xlsx
+++ b/public/template-import-faq-answers.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Intent</t>
   </si>
   <si>
     <t>Question</t>
+  </si>
+  <si>
+    <t>Language Code</t>
   </si>
 </sst>
 </file>
@@ -365,24 +368,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="20.77734375" customWidth="1"/>
+    <col min="1" max="3" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modify webhook, train network, and others
</commit_message>
<xml_diff>
--- a/public/template-import-faq-answers.xlsx
+++ b/public/template-import-faq-answers.xlsx
@@ -22,7 +22,7 @@
     <t>Question</t>
   </si>
   <si>
-    <t>Language Code</t>
+    <t>Locale</t>
   </si>
 </sst>
 </file>
@@ -370,9 +370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
modify template import faqs, faq answers, faq questions
</commit_message>
<xml_diff>
--- a/public/template-import-faq-answers.xlsx
+++ b/public/template-import-faq-answers.xlsx
@@ -14,15 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Intent</t>
   </si>
   <si>
-    <t>Question</t>
+    <t>Answer</t>
   </si>
   <si>
     <t>Locale</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
@@ -368,23 +371,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="20.77734375" customWidth="1"/>
+    <col min="1" max="4" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>